<commit_message>
Added profiling results after adding predict_array() method
</commit_message>
<xml_diff>
--- a/Method profiling/App profiling.xlsx
+++ b/Method profiling/App profiling.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>Lena-small.pgm (64k)</t>
   </si>
@@ -52,6 +52,12 @@
   </si>
   <si>
     <t>App version</t>
+  </si>
+  <si>
+    <t>Added predict_array() method and integrated searchTheWindow() with it - less calls of PGMImage.getPixel()</t>
+  </si>
+  <si>
+    <t>TOTAL OPTIMIZATION (original/optimized)</t>
   </si>
 </sst>
 </file>
@@ -146,7 +152,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -156,15 +162,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
@@ -173,7 +176,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -456,10 +468,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U12"/>
+  <dimension ref="A1:U15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K23" sqref="K23"/>
+      <selection activeCell="I24" sqref="I24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -470,10 +482,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="11" t="s">
         <v>9</v>
       </c>
       <c r="C1" s="8"/>
@@ -497,7 +509,7 @@
       <c r="U1" s="8"/>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A2" s="10"/>
+      <c r="A2" s="9"/>
       <c r="B2" s="8" t="s">
         <v>0</v>
       </c>
@@ -528,7 +540,7 @@
       <c r="U2" s="8"/>
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A3" s="12" t="s">
+      <c r="A3" s="7" t="s">
         <v>5</v>
       </c>
       <c r="B3" s="2">
@@ -593,7 +605,7 @@
       </c>
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A4" s="12"/>
+      <c r="A4" s="7"/>
       <c r="B4" s="8">
         <f>AVERAGE(B3:F3)</f>
         <v>14.462</v>
@@ -628,7 +640,7 @@
       <c r="U4" s="8"/>
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A5" s="10" t="s">
+      <c r="A5" s="9" t="s">
         <v>4</v>
       </c>
       <c r="B5">
@@ -693,7 +705,7 @@
       </c>
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A6" s="11"/>
+      <c r="A6" s="10"/>
       <c r="B6" s="8">
         <f>AVERAGE(B5:F5)</f>
         <v>13.8888</v>
@@ -728,7 +740,7 @@
       <c r="U6" s="8"/>
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A7" s="6" t="s">
+      <c r="A7" s="12" t="s">
         <v>6</v>
       </c>
       <c r="B7">
@@ -793,7 +805,7 @@
       </c>
     </row>
     <row r="8" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A8" s="7"/>
+      <c r="A8" s="13"/>
       <c r="B8" s="8">
         <f>AVERAGE(B7:F7)</f>
         <v>11.445400000000001</v>
@@ -828,7 +840,7 @@
       <c r="U8" s="8"/>
     </row>
     <row r="9" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A9" s="6" t="s">
+      <c r="A9" s="12" t="s">
         <v>7</v>
       </c>
       <c r="B9">
@@ -893,7 +905,7 @@
       </c>
     </row>
     <row r="10" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A10" s="7"/>
+      <c r="A10" s="13"/>
       <c r="B10" s="8">
         <f>AVERAGE(B9:F9)</f>
         <v>10.768400000000002</v>
@@ -928,7 +940,7 @@
       <c r="U10" s="8"/>
     </row>
     <row r="11" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A11" s="12" t="s">
+      <c r="A11" s="7" t="s">
         <v>8</v>
       </c>
       <c r="B11">
@@ -993,7 +1005,7 @@
       </c>
     </row>
     <row r="12" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A12" s="12"/>
+      <c r="A12" s="14"/>
       <c r="B12" s="8">
         <f>AVERAGE(B11:F11)</f>
         <v>5.5303999999999993</v>
@@ -1027,39 +1039,185 @@
       <c r="T12" s="8"/>
       <c r="U12" s="8"/>
     </row>
+    <row r="13" spans="1:21" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="B13">
+        <v>5.1130000000000004</v>
+      </c>
+      <c r="C13">
+        <v>5.157</v>
+      </c>
+      <c r="D13">
+        <v>5.2270000000000003</v>
+      </c>
+      <c r="E13">
+        <v>5.27</v>
+      </c>
+      <c r="F13" s="5">
+        <v>5.1180000000000003</v>
+      </c>
+      <c r="G13">
+        <v>21.106999999999999</v>
+      </c>
+      <c r="H13">
+        <v>21.152999999999999</v>
+      </c>
+      <c r="I13">
+        <v>21.146000000000001</v>
+      </c>
+      <c r="J13">
+        <v>21.187999999999999</v>
+      </c>
+      <c r="K13" s="5">
+        <v>21.370999999999999</v>
+      </c>
+      <c r="L13">
+        <v>33.747</v>
+      </c>
+      <c r="M13">
+        <v>33.634999999999998</v>
+      </c>
+      <c r="N13">
+        <v>33.851999999999997</v>
+      </c>
+      <c r="O13">
+        <v>33.637999999999998</v>
+      </c>
+      <c r="P13" s="5">
+        <v>34.003</v>
+      </c>
+      <c r="Q13">
+        <v>124.458</v>
+      </c>
+      <c r="R13">
+        <v>124.167</v>
+      </c>
+      <c r="S13">
+        <v>124.072</v>
+      </c>
+      <c r="T13">
+        <v>124.05800000000001</v>
+      </c>
+      <c r="U13" s="5">
+        <v>124.04600000000001</v>
+      </c>
+    </row>
+    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A14" s="12"/>
+      <c r="B14" s="8">
+        <f>AVERAGE(B13:F13)</f>
+        <v>5.1769999999999996</v>
+      </c>
+      <c r="C14" s="8"/>
+      <c r="D14" s="8"/>
+      <c r="E14" s="8"/>
+      <c r="F14" s="8"/>
+      <c r="G14" s="8">
+        <f>AVERAGE(G13:K13)</f>
+        <v>21.192999999999998</v>
+      </c>
+      <c r="H14" s="8"/>
+      <c r="I14" s="8"/>
+      <c r="J14" s="8"/>
+      <c r="K14" s="8"/>
+      <c r="L14" s="8">
+        <f>AVERAGE(L13:P13)</f>
+        <v>33.774999999999999</v>
+      </c>
+      <c r="M14" s="8"/>
+      <c r="N14" s="8"/>
+      <c r="O14" s="8"/>
+      <c r="P14" s="8"/>
+      <c r="Q14" s="8">
+        <f>AVERAGE(Q13:U13)</f>
+        <v>124.1602</v>
+      </c>
+      <c r="R14" s="8"/>
+      <c r="S14" s="8"/>
+      <c r="T14" s="8"/>
+      <c r="U14" s="8"/>
+    </row>
+    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A15" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B15" s="8">
+        <f>B4/B14</f>
+        <v>2.7935097546841803</v>
+      </c>
+      <c r="C15" s="8"/>
+      <c r="D15" s="8"/>
+      <c r="E15" s="8"/>
+      <c r="F15" s="8"/>
+      <c r="G15" s="8">
+        <f>G4/G14</f>
+        <v>2.8502996272354086</v>
+      </c>
+      <c r="H15" s="8"/>
+      <c r="I15" s="8"/>
+      <c r="J15" s="8"/>
+      <c r="K15" s="8"/>
+      <c r="L15" s="8">
+        <f>L4/L14</f>
+        <v>2.8228749074759438</v>
+      </c>
+      <c r="M15" s="8"/>
+      <c r="N15" s="8"/>
+      <c r="O15" s="8"/>
+      <c r="P15" s="8"/>
+      <c r="Q15" s="8">
+        <f>Q4/Q14</f>
+        <v>2.8088437357542917</v>
+      </c>
+      <c r="R15" s="8"/>
+      <c r="S15" s="8"/>
+      <c r="T15" s="8"/>
+      <c r="U15" s="8"/>
+    </row>
   </sheetData>
-  <mergeCells count="31">
-    <mergeCell ref="A11:A12"/>
-    <mergeCell ref="B12:F12"/>
-    <mergeCell ref="G12:K12"/>
-    <mergeCell ref="L12:P12"/>
-    <mergeCell ref="Q12:U12"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="B2:F2"/>
-    <mergeCell ref="A3:A4"/>
-    <mergeCell ref="B4:F4"/>
-    <mergeCell ref="G2:K2"/>
-    <mergeCell ref="A5:A6"/>
-    <mergeCell ref="B6:F6"/>
-    <mergeCell ref="G6:K6"/>
-    <mergeCell ref="L6:P6"/>
-    <mergeCell ref="Q6:U6"/>
+  <mergeCells count="40">
+    <mergeCell ref="B15:F15"/>
+    <mergeCell ref="G15:K15"/>
+    <mergeCell ref="L15:P15"/>
+    <mergeCell ref="Q15:U15"/>
+    <mergeCell ref="A13:A14"/>
+    <mergeCell ref="B14:F14"/>
+    <mergeCell ref="G14:K14"/>
+    <mergeCell ref="L14:P14"/>
+    <mergeCell ref="Q14:U14"/>
+    <mergeCell ref="A7:A8"/>
+    <mergeCell ref="B8:F8"/>
+    <mergeCell ref="G8:K8"/>
+    <mergeCell ref="L8:P8"/>
+    <mergeCell ref="Q8:U8"/>
+    <mergeCell ref="A9:A10"/>
+    <mergeCell ref="B10:F10"/>
+    <mergeCell ref="G10:K10"/>
+    <mergeCell ref="L10:P10"/>
+    <mergeCell ref="Q10:U10"/>
     <mergeCell ref="Q2:U2"/>
     <mergeCell ref="B1:U1"/>
     <mergeCell ref="G4:K4"/>
     <mergeCell ref="L4:P4"/>
     <mergeCell ref="Q4:U4"/>
     <mergeCell ref="L2:P2"/>
-    <mergeCell ref="A9:A10"/>
-    <mergeCell ref="B10:F10"/>
-    <mergeCell ref="G10:K10"/>
-    <mergeCell ref="L10:P10"/>
-    <mergeCell ref="Q10:U10"/>
-    <mergeCell ref="A7:A8"/>
-    <mergeCell ref="B8:F8"/>
-    <mergeCell ref="G8:K8"/>
-    <mergeCell ref="L8:P8"/>
-    <mergeCell ref="Q8:U8"/>
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="B6:F6"/>
+    <mergeCell ref="G6:K6"/>
+    <mergeCell ref="L6:P6"/>
+    <mergeCell ref="Q6:U6"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B2:F2"/>
+    <mergeCell ref="A3:A4"/>
+    <mergeCell ref="B4:F4"/>
+    <mergeCell ref="G2:K2"/>
+    <mergeCell ref="A11:A12"/>
+    <mergeCell ref="B12:F12"/>
+    <mergeCell ref="G12:K12"/>
+    <mergeCell ref="L12:P12"/>
+    <mergeCell ref="Q12:U12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Added profiling results after modifying searchTheWindow() Method (repeating vector variables)
</commit_message>
<xml_diff>
--- a/Method profiling/App profiling.xlsx
+++ b/Method profiling/App profiling.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17927"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18067"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>Lena-small.pgm (64k)</t>
   </si>
@@ -59,6 +59,9 @@
   <si>
     <t>TOTAL OPTIMIZATION (original/optimized)</t>
   </si>
+  <si>
+    <t>Modified searchTheWindow() method - using repeating vector variables</t>
+  </si>
 </sst>
 </file>
 
@@ -81,7 +84,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -148,11 +151,33 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -165,6 +190,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
@@ -185,8 +213,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -468,76 +499,76 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U15"/>
+  <dimension ref="A1:U17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I24" sqref="I24"/>
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="53.5703125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="48.85546875" style="1" customWidth="1"/>
     <col min="2" max="16" width="7" bestFit="1" customWidth="1"/>
     <col min="17" max="20" width="8" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="11" t="s">
+      <c r="B1" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8"/>
-      <c r="G1" s="8"/>
-      <c r="H1" s="8"/>
-      <c r="I1" s="8"/>
-      <c r="J1" s="8"/>
-      <c r="K1" s="8"/>
-      <c r="L1" s="8"/>
-      <c r="M1" s="8"/>
-      <c r="N1" s="8"/>
-      <c r="O1" s="8"/>
-      <c r="P1" s="8"/>
-      <c r="Q1" s="8"/>
-      <c r="R1" s="8"/>
-      <c r="S1" s="8"/>
-      <c r="T1" s="8"/>
-      <c r="U1" s="8"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
+      <c r="F1" s="9"/>
+      <c r="G1" s="9"/>
+      <c r="H1" s="9"/>
+      <c r="I1" s="9"/>
+      <c r="J1" s="9"/>
+      <c r="K1" s="9"/>
+      <c r="L1" s="9"/>
+      <c r="M1" s="9"/>
+      <c r="N1" s="9"/>
+      <c r="O1" s="9"/>
+      <c r="P1" s="9"/>
+      <c r="Q1" s="9"/>
+      <c r="R1" s="9"/>
+      <c r="S1" s="9"/>
+      <c r="T1" s="9"/>
+      <c r="U1" s="9"/>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A2" s="9"/>
-      <c r="B2" s="8" t="s">
+      <c r="A2" s="10"/>
+      <c r="B2" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="8"/>
-      <c r="D2" s="8"/>
-      <c r="E2" s="8"/>
-      <c r="F2" s="8"/>
-      <c r="G2" s="8" t="s">
+      <c r="C2" s="9"/>
+      <c r="D2" s="9"/>
+      <c r="E2" s="9"/>
+      <c r="F2" s="9"/>
+      <c r="G2" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="H2" s="8"/>
-      <c r="I2" s="8"/>
-      <c r="J2" s="8"/>
-      <c r="K2" s="8"/>
-      <c r="L2" s="8" t="s">
+      <c r="H2" s="9"/>
+      <c r="I2" s="9"/>
+      <c r="J2" s="9"/>
+      <c r="K2" s="9"/>
+      <c r="L2" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="M2" s="8"/>
-      <c r="N2" s="8"/>
-      <c r="O2" s="8"/>
-      <c r="P2" s="8"/>
-      <c r="Q2" s="8" t="s">
+      <c r="M2" s="9"/>
+      <c r="N2" s="9"/>
+      <c r="O2" s="9"/>
+      <c r="P2" s="9"/>
+      <c r="Q2" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="R2" s="8"/>
-      <c r="S2" s="8"/>
-      <c r="T2" s="8"/>
-      <c r="U2" s="8"/>
+      <c r="R2" s="9"/>
+      <c r="S2" s="9"/>
+      <c r="T2" s="9"/>
+      <c r="U2" s="9"/>
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
@@ -606,41 +637,41 @@
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A4" s="7"/>
-      <c r="B4" s="8">
+      <c r="B4" s="9">
         <f>AVERAGE(B3:F3)</f>
         <v>14.462</v>
       </c>
-      <c r="C4" s="8"/>
-      <c r="D4" s="8"/>
-      <c r="E4" s="8"/>
-      <c r="F4" s="8"/>
-      <c r="G4" s="8">
+      <c r="C4" s="9"/>
+      <c r="D4" s="9"/>
+      <c r="E4" s="9"/>
+      <c r="F4" s="9"/>
+      <c r="G4" s="9">
         <f>AVERAGE(G3:K3)</f>
         <v>60.406400000000005</v>
       </c>
-      <c r="H4" s="8"/>
-      <c r="I4" s="8"/>
-      <c r="J4" s="8"/>
-      <c r="K4" s="8"/>
-      <c r="L4" s="8">
+      <c r="H4" s="9"/>
+      <c r="I4" s="9"/>
+      <c r="J4" s="9"/>
+      <c r="K4" s="9"/>
+      <c r="L4" s="9">
         <f>AVERAGE(L3:P3)</f>
         <v>95.342600000000004</v>
       </c>
-      <c r="M4" s="8"/>
-      <c r="N4" s="8"/>
-      <c r="O4" s="8"/>
-      <c r="P4" s="8"/>
-      <c r="Q4" s="8">
+      <c r="M4" s="9"/>
+      <c r="N4" s="9"/>
+      <c r="O4" s="9"/>
+      <c r="P4" s="9"/>
+      <c r="Q4" s="9">
         <f>AVERAGE(Q3:U3)</f>
         <v>348.7466</v>
       </c>
-      <c r="R4" s="8"/>
-      <c r="S4" s="8"/>
-      <c r="T4" s="8"/>
-      <c r="U4" s="8"/>
+      <c r="R4" s="9"/>
+      <c r="S4" s="9"/>
+      <c r="T4" s="9"/>
+      <c r="U4" s="9"/>
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A5" s="9" t="s">
+      <c r="A5" s="10" t="s">
         <v>4</v>
       </c>
       <c r="B5">
@@ -705,42 +736,42 @@
       </c>
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A6" s="10"/>
-      <c r="B6" s="8">
+      <c r="A6" s="11"/>
+      <c r="B6" s="9">
         <f>AVERAGE(B5:F5)</f>
         <v>13.8888</v>
       </c>
-      <c r="C6" s="8"/>
-      <c r="D6" s="8"/>
-      <c r="E6" s="8"/>
-      <c r="F6" s="8"/>
-      <c r="G6" s="8">
+      <c r="C6" s="9"/>
+      <c r="D6" s="9"/>
+      <c r="E6" s="9"/>
+      <c r="F6" s="9"/>
+      <c r="G6" s="9">
         <f>AVERAGE(G5:K5)</f>
         <v>57.462199999999996</v>
       </c>
-      <c r="H6" s="8"/>
-      <c r="I6" s="8"/>
-      <c r="J6" s="8"/>
-      <c r="K6" s="8"/>
-      <c r="L6" s="8">
+      <c r="H6" s="9"/>
+      <c r="I6" s="9"/>
+      <c r="J6" s="9"/>
+      <c r="K6" s="9"/>
+      <c r="L6" s="9">
         <f>AVERAGE(L5:P5)</f>
         <v>90.661799999999999</v>
       </c>
-      <c r="M6" s="8"/>
-      <c r="N6" s="8"/>
-      <c r="O6" s="8"/>
-      <c r="P6" s="8"/>
-      <c r="Q6" s="8">
+      <c r="M6" s="9"/>
+      <c r="N6" s="9"/>
+      <c r="O6" s="9"/>
+      <c r="P6" s="9"/>
+      <c r="Q6" s="9">
         <f>AVERAGE(Q5:U5)</f>
         <v>332.86340000000007</v>
       </c>
-      <c r="R6" s="8"/>
-      <c r="S6" s="8"/>
-      <c r="T6" s="8"/>
-      <c r="U6" s="8"/>
+      <c r="R6" s="9"/>
+      <c r="S6" s="9"/>
+      <c r="T6" s="9"/>
+      <c r="U6" s="9"/>
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A7" s="12" t="s">
+      <c r="A7" s="13" t="s">
         <v>6</v>
       </c>
       <c r="B7">
@@ -805,42 +836,42 @@
       </c>
     </row>
     <row r="8" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A8" s="13"/>
-      <c r="B8" s="8">
+      <c r="A8" s="14"/>
+      <c r="B8" s="9">
         <f>AVERAGE(B7:F7)</f>
         <v>11.445400000000001</v>
       </c>
-      <c r="C8" s="8"/>
-      <c r="D8" s="8"/>
-      <c r="E8" s="8"/>
-      <c r="F8" s="8"/>
-      <c r="G8" s="8">
+      <c r="C8" s="9"/>
+      <c r="D8" s="9"/>
+      <c r="E8" s="9"/>
+      <c r="F8" s="9"/>
+      <c r="G8" s="9">
         <f>AVERAGE(G7:K7)</f>
         <v>46.411200000000001</v>
       </c>
-      <c r="H8" s="8"/>
-      <c r="I8" s="8"/>
-      <c r="J8" s="8"/>
-      <c r="K8" s="8"/>
-      <c r="L8" s="8">
+      <c r="H8" s="9"/>
+      <c r="I8" s="9"/>
+      <c r="J8" s="9"/>
+      <c r="K8" s="9"/>
+      <c r="L8" s="9">
         <f>AVERAGE(L7:P7)</f>
         <v>74.024000000000001</v>
       </c>
-      <c r="M8" s="8"/>
-      <c r="N8" s="8"/>
-      <c r="O8" s="8"/>
-      <c r="P8" s="8"/>
-      <c r="Q8" s="8">
+      <c r="M8" s="9"/>
+      <c r="N8" s="9"/>
+      <c r="O8" s="9"/>
+      <c r="P8" s="9"/>
+      <c r="Q8" s="9">
         <f>AVERAGE(Q7:U7)</f>
         <v>270.45079999999996</v>
       </c>
-      <c r="R8" s="8"/>
-      <c r="S8" s="8"/>
-      <c r="T8" s="8"/>
-      <c r="U8" s="8"/>
+      <c r="R8" s="9"/>
+      <c r="S8" s="9"/>
+      <c r="T8" s="9"/>
+      <c r="U8" s="9"/>
     </row>
     <row r="9" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A9" s="12" t="s">
+      <c r="A9" s="13" t="s">
         <v>7</v>
       </c>
       <c r="B9">
@@ -905,39 +936,39 @@
       </c>
     </row>
     <row r="10" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A10" s="13"/>
-      <c r="B10" s="8">
+      <c r="A10" s="14"/>
+      <c r="B10" s="9">
         <f>AVERAGE(B9:F9)</f>
         <v>10.768400000000002</v>
       </c>
-      <c r="C10" s="8"/>
-      <c r="D10" s="8"/>
-      <c r="E10" s="8"/>
-      <c r="F10" s="8"/>
-      <c r="G10" s="8">
+      <c r="C10" s="9"/>
+      <c r="D10" s="9"/>
+      <c r="E10" s="9"/>
+      <c r="F10" s="9"/>
+      <c r="G10" s="9">
         <f>AVERAGE(G9:K9)</f>
         <v>42.3934</v>
       </c>
-      <c r="H10" s="8"/>
-      <c r="I10" s="8"/>
-      <c r="J10" s="8"/>
-      <c r="K10" s="8"/>
-      <c r="L10" s="8">
+      <c r="H10" s="9"/>
+      <c r="I10" s="9"/>
+      <c r="J10" s="9"/>
+      <c r="K10" s="9"/>
+      <c r="L10" s="9">
         <f>AVERAGE(L9:P9)</f>
         <v>69.085999999999999</v>
       </c>
-      <c r="M10" s="8"/>
-      <c r="N10" s="8"/>
-      <c r="O10" s="8"/>
-      <c r="P10" s="8"/>
-      <c r="Q10" s="8">
+      <c r="M10" s="9"/>
+      <c r="N10" s="9"/>
+      <c r="O10" s="9"/>
+      <c r="P10" s="9"/>
+      <c r="Q10" s="9">
         <f>AVERAGE(Q9:U9)</f>
         <v>249.40060000000003</v>
       </c>
-      <c r="R10" s="8"/>
-      <c r="S10" s="8"/>
-      <c r="T10" s="8"/>
-      <c r="U10" s="8"/>
+      <c r="R10" s="9"/>
+      <c r="S10" s="9"/>
+      <c r="T10" s="9"/>
+      <c r="U10" s="9"/>
     </row>
     <row r="11" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
@@ -1005,42 +1036,42 @@
       </c>
     </row>
     <row r="12" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A12" s="14"/>
-      <c r="B12" s="8">
+      <c r="A12" s="8"/>
+      <c r="B12" s="9">
         <f>AVERAGE(B11:F11)</f>
         <v>5.5303999999999993</v>
       </c>
-      <c r="C12" s="8"/>
-      <c r="D12" s="8"/>
-      <c r="E12" s="8"/>
-      <c r="F12" s="8"/>
-      <c r="G12" s="8">
+      <c r="C12" s="9"/>
+      <c r="D12" s="9"/>
+      <c r="E12" s="9"/>
+      <c r="F12" s="9"/>
+      <c r="G12" s="9">
         <f>AVERAGE(G11:K11)</f>
         <v>22.591799999999999</v>
       </c>
-      <c r="H12" s="8"/>
-      <c r="I12" s="8"/>
-      <c r="J12" s="8"/>
-      <c r="K12" s="8"/>
-      <c r="L12" s="8">
+      <c r="H12" s="9"/>
+      <c r="I12" s="9"/>
+      <c r="J12" s="9"/>
+      <c r="K12" s="9"/>
+      <c r="L12" s="9">
         <f>AVERAGE(L11:P11)</f>
         <v>35.877800000000001</v>
       </c>
-      <c r="M12" s="8"/>
-      <c r="N12" s="8"/>
-      <c r="O12" s="8"/>
-      <c r="P12" s="8"/>
-      <c r="Q12" s="8">
+      <c r="M12" s="9"/>
+      <c r="N12" s="9"/>
+      <c r="O12" s="9"/>
+      <c r="P12" s="9"/>
+      <c r="Q12" s="9">
         <f>AVERAGE(Q11:U11)</f>
         <v>131.6908</v>
       </c>
-      <c r="R12" s="8"/>
-      <c r="S12" s="8"/>
-      <c r="T12" s="8"/>
-      <c r="U12" s="8"/>
+      <c r="R12" s="9"/>
+      <c r="S12" s="9"/>
+      <c r="T12" s="9"/>
+      <c r="U12" s="9"/>
     </row>
     <row r="13" spans="1:21" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="12" t="s">
+      <c r="A13" s="13" t="s">
         <v>11</v>
       </c>
       <c r="B13">
@@ -1105,88 +1136,142 @@
       </c>
     </row>
     <row r="14" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A14" s="12"/>
-      <c r="B14" s="8">
+      <c r="A14" s="13"/>
+      <c r="B14" s="9">
         <f>AVERAGE(B13:F13)</f>
         <v>5.1769999999999996</v>
       </c>
-      <c r="C14" s="8"/>
-      <c r="D14" s="8"/>
-      <c r="E14" s="8"/>
-      <c r="F14" s="8"/>
-      <c r="G14" s="8">
+      <c r="C14" s="9"/>
+      <c r="D14" s="9"/>
+      <c r="E14" s="9"/>
+      <c r="F14" s="9"/>
+      <c r="G14" s="9">
         <f>AVERAGE(G13:K13)</f>
         <v>21.192999999999998</v>
       </c>
-      <c r="H14" s="8"/>
-      <c r="I14" s="8"/>
-      <c r="J14" s="8"/>
-      <c r="K14" s="8"/>
-      <c r="L14" s="8">
+      <c r="H14" s="9"/>
+      <c r="I14" s="9"/>
+      <c r="J14" s="9"/>
+      <c r="K14" s="9"/>
+      <c r="L14" s="9">
         <f>AVERAGE(L13:P13)</f>
         <v>33.774999999999999</v>
       </c>
-      <c r="M14" s="8"/>
-      <c r="N14" s="8"/>
-      <c r="O14" s="8"/>
-      <c r="P14" s="8"/>
-      <c r="Q14" s="8">
+      <c r="M14" s="9"/>
+      <c r="N14" s="9"/>
+      <c r="O14" s="9"/>
+      <c r="P14" s="9"/>
+      <c r="Q14" s="9">
         <f>AVERAGE(Q13:U13)</f>
         <v>124.1602</v>
       </c>
-      <c r="R14" s="8"/>
-      <c r="S14" s="8"/>
-      <c r="T14" s="8"/>
-      <c r="U14" s="8"/>
+      <c r="R14" s="9"/>
+      <c r="S14" s="9"/>
+      <c r="T14" s="9"/>
+      <c r="U14" s="9"/>
     </row>
     <row r="15" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A15" s="6" t="s">
+      <c r="A15" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="B15">
+        <v>4.63</v>
+      </c>
+      <c r="C15">
+        <v>4.7960000000000003</v>
+      </c>
+      <c r="D15">
+        <v>4.8079999999999998</v>
+      </c>
+      <c r="E15">
+        <v>4.7350000000000003</v>
+      </c>
+      <c r="F15" s="3">
+        <v>4.6680000000000001</v>
+      </c>
+      <c r="K15" s="3"/>
+      <c r="P15" s="3"/>
+      <c r="U15" s="3"/>
+    </row>
+    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A16" s="16"/>
+      <c r="B16" s="9">
+        <f>AVERAGE(B15:F15)</f>
+        <v>4.7274000000000003</v>
+      </c>
+      <c r="C16" s="9"/>
+      <c r="D16" s="9"/>
+      <c r="E16" s="9"/>
+      <c r="F16" s="9"/>
+      <c r="G16" s="9"/>
+      <c r="H16" s="9"/>
+      <c r="I16" s="9"/>
+      <c r="J16" s="9"/>
+      <c r="K16" s="9"/>
+      <c r="L16" s="9"/>
+      <c r="M16" s="9"/>
+      <c r="N16" s="9"/>
+      <c r="O16" s="9"/>
+      <c r="P16" s="9"/>
+      <c r="Q16" s="9"/>
+      <c r="R16" s="9"/>
+      <c r="S16" s="9"/>
+      <c r="T16" s="9"/>
+      <c r="U16" s="9"/>
+    </row>
+    <row r="17" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A17" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="B15" s="8">
-        <f>B4/B14</f>
-        <v>2.7935097546841803</v>
-      </c>
-      <c r="C15" s="8"/>
-      <c r="D15" s="8"/>
-      <c r="E15" s="8"/>
-      <c r="F15" s="8"/>
-      <c r="G15" s="8">
+      <c r="B17" s="9">
+        <f>B4/B16</f>
+        <v>3.05918686804586</v>
+      </c>
+      <c r="C17" s="9"/>
+      <c r="D17" s="9"/>
+      <c r="E17" s="9"/>
+      <c r="F17" s="9"/>
+      <c r="G17" s="9">
         <f>G4/G14</f>
         <v>2.8502996272354086</v>
       </c>
-      <c r="H15" s="8"/>
-      <c r="I15" s="8"/>
-      <c r="J15" s="8"/>
-      <c r="K15" s="8"/>
-      <c r="L15" s="8">
+      <c r="H17" s="9"/>
+      <c r="I17" s="9"/>
+      <c r="J17" s="9"/>
+      <c r="K17" s="9"/>
+      <c r="L17" s="9">
         <f>L4/L14</f>
         <v>2.8228749074759438</v>
       </c>
-      <c r="M15" s="8"/>
-      <c r="N15" s="8"/>
-      <c r="O15" s="8"/>
-      <c r="P15" s="8"/>
-      <c r="Q15" s="8">
+      <c r="M17" s="9"/>
+      <c r="N17" s="9"/>
+      <c r="O17" s="9"/>
+      <c r="P17" s="9"/>
+      <c r="Q17" s="9">
         <f>Q4/Q14</f>
         <v>2.8088437357542917</v>
       </c>
-      <c r="R15" s="8"/>
-      <c r="S15" s="8"/>
-      <c r="T15" s="8"/>
-      <c r="U15" s="8"/>
+      <c r="R17" s="9"/>
+      <c r="S17" s="9"/>
+      <c r="T17" s="9"/>
+      <c r="U17" s="9"/>
     </row>
   </sheetData>
-  <mergeCells count="40">
-    <mergeCell ref="B15:F15"/>
-    <mergeCell ref="G15:K15"/>
-    <mergeCell ref="L15:P15"/>
-    <mergeCell ref="Q15:U15"/>
+  <mergeCells count="45">
+    <mergeCell ref="B17:F17"/>
+    <mergeCell ref="G17:K17"/>
+    <mergeCell ref="L17:P17"/>
+    <mergeCell ref="Q17:U17"/>
     <mergeCell ref="A13:A14"/>
     <mergeCell ref="B14:F14"/>
     <mergeCell ref="G14:K14"/>
     <mergeCell ref="L14:P14"/>
     <mergeCell ref="Q14:U14"/>
+    <mergeCell ref="A15:A16"/>
+    <mergeCell ref="B16:F16"/>
+    <mergeCell ref="G16:K16"/>
+    <mergeCell ref="L16:P16"/>
+    <mergeCell ref="Q16:U16"/>
     <mergeCell ref="A7:A8"/>
     <mergeCell ref="B8:F8"/>
     <mergeCell ref="G8:K8"/>

</xml_diff>